<commit_message>
Updated Date on Orders
</commit_message>
<xml_diff>
--- a/Project 4/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Project 4/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\University\Semester 2\CMPG 323\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C519AD8-3C41-460B-B76B-FF9FE2FF5E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB457047-C743-4430-BF1E-3C5137365BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11616" yWindow="5580" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1719,7 +1719,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E16" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,9 +1761,6 @@
       <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1784,7 +1781,7 @@
         <v>100055</v>
       </c>
       <c r="B4" s="1">
-        <v>42883</v>
+        <v>41828</v>
       </c>
       <c r="C4">
         <v>19420</v>

</xml_diff>

<commit_message>
Added Choise to select mechanism
</commit_message>
<xml_diff>
--- a/Project 4/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Project 4/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\University\Semester 2\CMPG 323\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB457047-C743-4430-BF1E-3C5137365BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF505A-4822-445E-9B5F-3228A8780BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11616" yWindow="5580" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11616" yWindow="5580" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
@@ -782,6 +782,9 @@
       <c r="E2">
         <v>5723177115</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -799,6 +802,9 @@
       <c r="E3">
         <v>9041993848</v>
       </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -816,6 +822,9 @@
       <c r="E4">
         <v>3738283528</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -833,6 +842,9 @@
       <c r="E5">
         <v>6447102299</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -849,6 +861,9 @@
       </c>
       <c r="E6">
         <v>1878764468</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1718,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
@@ -1954,7 +1969,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E2:E7"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,6 +2011,9 @@
       <c r="D2">
         <v>950</v>
       </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2010,6 +2028,9 @@
       <c r="D3">
         <v>61</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2024,6 +2045,9 @@
       <c r="D4">
         <v>281</v>
       </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2038,6 +2062,9 @@
       <c r="D5">
         <v>502</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2052,6 +2079,9 @@
       <c r="D6">
         <v>621</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2066,6 +2096,9 @@
       <c r="D7">
         <v>765</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2080,6 +2113,9 @@
       <c r="D8">
         <v>709</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2094,6 +2130,9 @@
       <c r="D9">
         <v>485</v>
       </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2108,6 +2147,9 @@
       <c r="D10">
         <v>158</v>
       </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2122,6 +2164,9 @@
       <c r="D11">
         <v>485</v>
       </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2135,6 +2180,9 @@
       </c>
       <c r="D12">
         <v>322</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>